<commit_message>
Schematics, BoM updated. New project added - scale_ltc6915
</commit_message>
<xml_diff>
--- a/design/scale_hx711/scale_hx711_BoM.xlsx
+++ b/design/scale_hx711/scale_hx711_BoM.xlsx
@@ -20,15 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="130">
-  <si>
-    <t xml:space="preserve">nrf_scale_hx711 Bill Of Materials (BoM)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="155">
+  <si>
+    <t xml:space="preserve">Source:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/shubham/IoTReady/nrf_scale/weighing_scale_nrf/design/scale_hx711/scale_hx711.sch</t>
   </si>
   <si>
     <t xml:space="preserve">Date:</t>
   </si>
   <si>
-    <t xml:space="preserve">Fri Mar  6 13:02:03 2020</t>
+    <t xml:space="preserve">Fri Mar  6 21:36:16 2020</t>
   </si>
   <si>
     <t xml:space="preserve">Tool:</t>
@@ -64,7 +67,7 @@
     <t xml:space="preserve">Battery_Cell</t>
   </si>
   <si>
-    <t xml:space="preserve">Connector_JST:JST_XH_B2B-XH-AM_1x02_P2.50mm_Vertical</t>
+    <t xml:space="preserve">Connector_JST:JST_PH_B2B-PH-K_1x02_P2.00mm_Vertical</t>
   </si>
   <si>
     <t xml:space="preserve">C1</t>
@@ -163,6 +166,12 @@
     <t xml:space="preserve">C22</t>
   </si>
   <si>
+    <t xml:space="preserve">4.7uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~</t>
+  </si>
+  <si>
     <t xml:space="preserve">C23</t>
   </si>
   <si>
@@ -175,6 +184,33 @@
     <t xml:space="preserve">C26</t>
   </si>
   <si>
+    <t xml:space="preserve">C27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C32</t>
+  </si>
+  <si>
     <t xml:space="preserve">D1</t>
   </si>
   <si>
@@ -193,15 +229,15 @@
     <t xml:space="preserve">Diode_SMD:D_SOD-323_HandSoldering</t>
   </si>
   <si>
-    <t xml:space="preserve">~</t>
-  </si>
-  <si>
     <t xml:space="preserve">D3</t>
   </si>
   <si>
     <t xml:space="preserve">D4</t>
   </si>
   <si>
+    <t xml:space="preserve">D5</t>
+  </si>
+  <si>
     <t xml:space="preserve">EINK1</t>
   </si>
   <si>
@@ -226,7 +262,7 @@
     <t xml:space="preserve">Conn_02x03_Odd_Even</t>
   </si>
   <si>
-    <t xml:space="preserve">sense_fp:PinHeader_2x03_P2.54mm_Vertical</t>
+    <t xml:space="preserve">Connector_PinHeader_2.00mm:PinHeader_2x03_P2.00mm_Vertical</t>
   </si>
   <si>
     <t xml:space="preserve">J3</t>
@@ -235,7 +271,7 @@
     <t xml:space="preserve">Load cell</t>
   </si>
   <si>
-    <t xml:space="preserve">Connector_JST:JST_EH_B4B-EH-A_1x04_P2.50mm_Vertical</t>
+    <t xml:space="preserve">Connector_JST:JST_PH_B4B-PH-K_1x04_P2.00mm_Vertical</t>
   </si>
   <si>
     <t xml:space="preserve">L1</t>
@@ -262,6 +298,12 @@
     <t xml:space="preserve">Footprint_nrf_scale:L_3.5x3.0mm_CD30D22</t>
   </si>
   <si>
+    <t xml:space="preserve">L4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3uH</t>
+  </si>
+  <si>
     <t xml:space="preserve">MK1</t>
   </si>
   <si>
@@ -343,13 +385,31 @@
     <t xml:space="preserve">R9</t>
   </si>
   <si>
+    <t xml:space="preserve">R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.9k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13</t>
+  </si>
+  <si>
     <t xml:space="preserve">SW1</t>
   </si>
   <si>
     <t xml:space="preserve">SW_SPST</t>
   </si>
   <si>
-    <t xml:space="preserve">sense_fp:SW_PUSH_6mm</t>
+    <t xml:space="preserve">Footprint_nrf_scale:SMD Tactile Switch_3x6x2.5mm</t>
   </si>
   <si>
     <t xml:space="preserve">SW2</t>
@@ -358,7 +418,7 @@
     <t xml:space="preserve">ON/OFF switch</t>
   </si>
   <si>
-    <t xml:space="preserve">sense_fp:SlideSwitch_1P2T_Straight</t>
+    <t xml:space="preserve">Footprint_nrf_scale:Slide Switch SMD 2P2T _6pins</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
@@ -401,6 +461,21 @@
   </si>
   <si>
     <t xml:space="preserve">Package_SO:SOIC-16_3.9x9.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM2703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP2985-5.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.ti.com/lit/ds/symlink/lp2985.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Y1</t>
@@ -419,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -439,12 +514,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -489,13 +558,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -519,16 +584,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="65.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.13"/>
@@ -536,377 +601,384 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,13 +986,13 @@
         <v>58</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,13 +1000,13 @@
         <v>59</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -945,142 +1017,160 @@
         <v>61</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>62</v>
+        <v>33</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>17</v>
+        <v>68</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>76</v>
+        <v>68</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>79</v>
+        <v>68</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>88</v>
@@ -1088,35 +1178,32 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>96</v>
@@ -1124,7 +1211,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>95</v>
@@ -1135,10 +1222,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>96</v>
@@ -1146,10 +1233,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="2" t="n">
-        <v>0.47</v>
+        <v>99</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>95</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>96</v>
@@ -1157,135 +1244,292 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="B56" s="0" t="s">
+        <v>101</v>
+      </c>
       <c r="C56" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="2" t="n">
-        <v>100</v>
-      </c>
       <c r="C57" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B58" s="2" t="n">
-        <v>100</v>
+      <c r="B58" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B59" s="2" t="n">
-        <v>100</v>
+        <v>108</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="B63" s="0" t="s">
-        <v>117</v>
+      <c r="B63" s="1" t="n">
+        <v>0.47</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>121</v>
+        <v>117</v>
+      </c>
+      <c r="B64" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>125</v>
+        <v>118</v>
+      </c>
+      <c r="B65" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B72" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C72" s="0" t="s">
         <v>129</v>
       </c>
     </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
BOMs, schematics updated, scale_ltc6915 PCB Design complete.
</commit_message>
<xml_diff>
--- a/design/scale_hx711/scale_hx711_BoM.xlsx
+++ b/design/scale_hx711/scale_hx711_BoM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="164">
   <si>
     <t xml:space="preserve">Source:</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Date:</t>
   </si>
   <si>
-    <t xml:space="preserve">Fri Mar  6 21:36:16 2020</t>
+    <t xml:space="preserve">Tue Mar 10 15:40:08 2020</t>
   </si>
   <si>
     <t xml:space="preserve">Tool:</t>
@@ -274,6 +274,15 @@
     <t xml:space="preserve">Connector_JST:JST_PH_B4B-PH-K_1x04_P2.00mm_Vertical</t>
   </si>
   <si>
+    <t xml:space="preserve">J4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conn_01x04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector_PinHeader_2.00mm:PinHeader_1x04_P2.00mm_Vertical</t>
+  </si>
+  <si>
     <t xml:space="preserve">L1</t>
   </si>
   <si>
@@ -346,6 +355,9 @@
     <t xml:space="preserve">http://www.fairchildsemi.com/ds/BC/BC557.pdf</t>
   </si>
   <si>
+    <t xml:space="preserve">Q4</t>
+  </si>
+  <si>
     <t xml:space="preserve">R1</t>
   </si>
   <si>
@@ -373,12 +385,21 @@
     <t xml:space="preserve">R5</t>
   </si>
   <si>
+    <t xml:space="preserve">Resistor_SMD:R_1206_3216Metric</t>
+  </si>
+  <si>
     <t xml:space="preserve">R6</t>
   </si>
   <si>
+    <t xml:space="preserve">4.7k</t>
+  </si>
+  <si>
     <t xml:space="preserve">R7</t>
   </si>
   <si>
+    <t xml:space="preserve">24k</t>
+  </si>
+  <si>
     <t xml:space="preserve">R8</t>
   </si>
   <si>
@@ -401,6 +422,12 @@
   </si>
   <si>
     <t xml:space="preserve">R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15</t>
   </si>
   <si>
     <t xml:space="preserve">SW1</t>
@@ -584,7 +611,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -630,7 +657,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,18 +1189,21 @@
         <v>85</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>18</v>
+        <v>86</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1195,18 +1225,18 @@
         <v>93</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,43 +1244,43 @@
         <v>97</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>95</v>
-      </c>
       <c r="C54" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,21 +1291,18 @@
         <v>104</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,6 +1313,9 @@
         <v>109</v>
       </c>
       <c r="C59" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" s="0" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1294,239 +1324,283 @@
         <v>111</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="B61" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="C61" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B63" s="1" t="n">
-        <v>0.47</v>
+        <v>117</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>113</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B64" s="1" t="n">
-        <v>100</v>
+        <v>118</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>100</v>
+        <v>0.47</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B66" s="1" t="n">
-        <v>100</v>
+        <v>122</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>123</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B67" s="1" t="n">
-        <v>100</v>
+        <v>124</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>125</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
+      </c>
+      <c r="B68" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
+      </c>
+      <c r="B69" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="0" t="s">
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="B81" s="0" t="s">
         <v>154</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>